<commit_message>
v1.1 pre-release - 修改数据结构 - excel 创建 csv - xlrd 读excel取代 openpyxl 速度快两倍 - 修改bookClicked的逻辑
</commit_message>
<xml_diff>
--- a/PyQt5_GUI/RemV_Package/lib/res/word_Repository/ErrorBook.xlsx
+++ b/PyQt5_GUI/RemV_Package/lib/res/word_Repository/ErrorBook.xlsx
@@ -1,34 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Armand\PycharmProjects\RemV\PyQt5_GUI\RemV_Package\lib\res\word_Repository\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFC58C9-B8D4-45D2-9AFA-18B67ABAD68F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RemV_ErrorBook" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Book" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -44,15 +59,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -340,19 +364,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>